<commit_message>
reran script with new labels
</commit_message>
<xml_diff>
--- a/metadata/questionLabels.xlsx
+++ b/metadata/questionLabels.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="881">
   <si>
     <t xml:space="preserve">Original position</t>
   </si>
@@ -1913,6 +1913,12 @@
     <t xml:space="preserve">Se että saisin itse tartunnan..</t>
   </si>
   <si>
+    <t xml:space="preserve">The fact that I would get infected myself ..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I would get infected myself ..</t>
+  </si>
+  <si>
     <t xml:space="preserve">risk_fear_contagion_self</t>
   </si>
   <si>
@@ -1931,6 +1937,12 @@
     <t xml:space="preserve">Se että läheiseni saisi tartunnan..</t>
   </si>
   <si>
+    <t xml:space="preserve">That my loved one would get infected...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loved one would get infected...</t>
+  </si>
+  <si>
     <t xml:space="preserve">risk_fear_contagion_others</t>
   </si>
   <si>
@@ -1947,6 +1959,12 @@
   </si>
   <si>
     <t xml:space="preserve">Koronaviruksen leviämisen estämiseksi tehtyjen toimien seuraukset yhteiskunnassa..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consequences of measures taken to prevent the spread of the coronavirus...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measures taken to prevent the spread</t>
   </si>
   <si>
     <t xml:space="preserve">risk_fear_restrictions</t>
@@ -6791,19 +6809,19 @@
         <v>632</v>
       </c>
       <c r="D71" t="s">
-        <v>626</v>
+        <v>633</v>
       </c>
       <c r="E71" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="F71" t="s">
         <v>597</v>
       </c>
       <c r="G71" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="H71" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="I71" t="s">
         <v>285</v>
@@ -6833,33 +6851,33 @@
       <c r="T71"/>
       <c r="U71"/>
       <c r="V71" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B72" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="C72" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="D72" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
       <c r="E72" t="s">
-        <v>626</v>
+        <v>642</v>
       </c>
       <c r="F72" t="s">
         <v>597</v>
       </c>
       <c r="G72" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="H72" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="I72" t="s">
         <v>285</v>
@@ -6889,42 +6907,42 @@
       <c r="T72"/>
       <c r="U72"/>
       <c r="V72" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="B73" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="C73" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="D73" t="s">
-        <v>626</v>
+        <v>649</v>
       </c>
       <c r="E73" t="s">
-        <v>626</v>
+        <v>650</v>
       </c>
       <c r="F73" t="s">
         <v>597</v>
       </c>
       <c r="G73" t="s">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="H73" t="s">
-        <v>646</v>
+        <v>652</v>
       </c>
       <c r="I73" t="s">
         <v>285</v>
       </c>
       <c r="J73" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="K73" t="s">
-        <v>648</v>
+        <v>654</v>
       </c>
       <c r="L73" t="s">
         <v>602</v>
@@ -6945,33 +6963,33 @@
       <c r="T73"/>
       <c r="U73"/>
       <c r="V73" t="s">
-        <v>649</v>
+        <v>655</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="B74" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="C74" t="s">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="D74" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="E74" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="F74" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="G74" t="s">
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="H74" t="s">
-        <v>657</v>
+        <v>663</v>
       </c>
       <c r="I74" t="s">
         <v>238</v>
@@ -6980,13 +6998,13 @@
         <v>128</v>
       </c>
       <c r="K74" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="L74" t="s">
         <v>130</v>
       </c>
       <c r="M74" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="N74" t="s">
         <v>51</v>
@@ -7001,33 +7019,33 @@
       <c r="T74"/>
       <c r="U74"/>
       <c r="V74" t="s">
-        <v>660</v>
+        <v>666</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>667</v>
+      </c>
+      <c r="B75" t="s">
+        <v>668</v>
+      </c>
+      <c r="C75" t="s">
+        <v>669</v>
+      </c>
+      <c r="D75" t="s">
+        <v>670</v>
+      </c>
+      <c r="E75" t="s">
+        <v>671</v>
+      </c>
+      <c r="F75" t="s">
         <v>661</v>
       </c>
-      <c r="B75" t="s">
-        <v>662</v>
-      </c>
-      <c r="C75" t="s">
-        <v>663</v>
-      </c>
-      <c r="D75" t="s">
-        <v>664</v>
-      </c>
-      <c r="E75" t="s">
-        <v>665</v>
-      </c>
-      <c r="F75" t="s">
-        <v>655</v>
-      </c>
       <c r="G75" t="s">
-        <v>666</v>
+        <v>672</v>
       </c>
       <c r="H75" t="s">
-        <v>667</v>
+        <v>673</v>
       </c>
       <c r="I75" t="s">
         <v>238</v>
@@ -7036,13 +7054,13 @@
         <v>128</v>
       </c>
       <c r="K75" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="L75" t="s">
         <v>130</v>
       </c>
       <c r="M75" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="N75" t="s">
         <v>51</v>
@@ -7057,33 +7075,33 @@
       <c r="T75"/>
       <c r="U75"/>
       <c r="V75" t="s">
-        <v>668</v>
+        <v>674</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>669</v>
+        <v>675</v>
       </c>
       <c r="B76" t="s">
-        <v>670</v>
+        <v>676</v>
       </c>
       <c r="C76" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="D76" t="s">
-        <v>672</v>
+        <v>678</v>
       </c>
       <c r="E76" t="s">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="F76" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="G76" t="s">
-        <v>674</v>
+        <v>680</v>
       </c>
       <c r="H76" t="s">
-        <v>675</v>
+        <v>681</v>
       </c>
       <c r="I76" t="s">
         <v>238</v>
@@ -7092,13 +7110,13 @@
         <v>128</v>
       </c>
       <c r="K76" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="L76" t="s">
         <v>130</v>
       </c>
       <c r="M76" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="N76" t="s">
         <v>51</v>
@@ -7113,33 +7131,33 @@
       <c r="T76"/>
       <c r="U76"/>
       <c r="V76" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>677</v>
+        <v>683</v>
       </c>
       <c r="B77" t="s">
-        <v>678</v>
+        <v>684</v>
       </c>
       <c r="C77" t="s">
-        <v>679</v>
+        <v>685</v>
       </c>
       <c r="D77" t="s">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="E77" t="s">
-        <v>681</v>
+        <v>687</v>
       </c>
       <c r="F77" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="G77" t="s">
-        <v>682</v>
+        <v>688</v>
       </c>
       <c r="H77" t="s">
-        <v>683</v>
+        <v>689</v>
       </c>
       <c r="I77" t="s">
         <v>238</v>
@@ -7148,13 +7166,13 @@
         <v>128</v>
       </c>
       <c r="K77" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="L77" t="s">
         <v>130</v>
       </c>
       <c r="M77" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="N77" t="s">
         <v>51</v>
@@ -7169,33 +7187,33 @@
       <c r="T77"/>
       <c r="U77"/>
       <c r="V77" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>685</v>
+        <v>691</v>
       </c>
       <c r="B78" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
       <c r="C78" t="s">
-        <v>687</v>
+        <v>693</v>
       </c>
       <c r="D78" t="s">
-        <v>688</v>
+        <v>694</v>
       </c>
       <c r="E78" t="s">
-        <v>689</v>
+        <v>695</v>
       </c>
       <c r="F78" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="G78" t="s">
-        <v>690</v>
+        <v>696</v>
       </c>
       <c r="H78" t="s">
-        <v>691</v>
+        <v>697</v>
       </c>
       <c r="I78" t="s">
         <v>238</v>
@@ -7204,13 +7222,13 @@
         <v>128</v>
       </c>
       <c r="K78" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="L78" t="s">
         <v>130</v>
       </c>
       <c r="M78" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="N78" t="s">
         <v>51</v>
@@ -7225,33 +7243,33 @@
       <c r="T78"/>
       <c r="U78"/>
       <c r="V78" t="s">
-        <v>692</v>
+        <v>698</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>693</v>
+        <v>699</v>
       </c>
       <c r="B79" t="s">
-        <v>694</v>
+        <v>700</v>
       </c>
       <c r="C79" t="s">
-        <v>695</v>
+        <v>701</v>
       </c>
       <c r="D79" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
       <c r="E79" t="s">
-        <v>697</v>
+        <v>703</v>
       </c>
       <c r="F79" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="G79" t="s">
-        <v>698</v>
+        <v>704</v>
       </c>
       <c r="H79" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
       <c r="I79" t="s">
         <v>238</v>
@@ -7260,13 +7278,13 @@
         <v>128</v>
       </c>
       <c r="K79" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="L79" t="s">
         <v>130</v>
       </c>
       <c r="M79" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="N79" t="s">
         <v>51</v>
@@ -7281,48 +7299,48 @@
       <c r="T79"/>
       <c r="U79"/>
       <c r="V79" t="s">
-        <v>700</v>
+        <v>706</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>701</v>
+        <v>707</v>
       </c>
       <c r="B80" t="s">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c r="C80" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="D80" t="s">
-        <v>704</v>
+        <v>710</v>
       </c>
       <c r="E80" t="s">
-        <v>705</v>
+        <v>711</v>
       </c>
       <c r="F80" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G80" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
       <c r="H80" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="I80" t="s">
         <v>238</v>
       </c>
       <c r="J80" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K80" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L80" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M80" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N80" t="s">
         <v>51</v>
@@ -7337,48 +7355,48 @@
       <c r="T80"/>
       <c r="U80"/>
       <c r="V80" t="s">
-        <v>713</v>
+        <v>719</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>714</v>
+        <v>720</v>
       </c>
       <c r="B81" t="s">
-        <v>715</v>
+        <v>721</v>
       </c>
       <c r="C81" t="s">
-        <v>716</v>
+        <v>722</v>
       </c>
       <c r="D81" t="s">
-        <v>717</v>
+        <v>723</v>
       </c>
       <c r="E81" t="s">
-        <v>717</v>
+        <v>723</v>
       </c>
       <c r="F81" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G81" t="s">
-        <v>718</v>
+        <v>724</v>
       </c>
       <c r="H81" t="s">
-        <v>719</v>
+        <v>725</v>
       </c>
       <c r="I81" t="s">
         <v>238</v>
       </c>
       <c r="J81" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K81" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L81" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M81" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N81" t="s">
         <v>51</v>
@@ -7393,48 +7411,48 @@
       <c r="T81"/>
       <c r="U81"/>
       <c r="V81" t="s">
-        <v>720</v>
+        <v>726</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>721</v>
+        <v>727</v>
       </c>
       <c r="B82" t="s">
-        <v>722</v>
+        <v>728</v>
       </c>
       <c r="C82" t="s">
-        <v>723</v>
+        <v>729</v>
       </c>
       <c r="D82" t="s">
-        <v>724</v>
+        <v>730</v>
       </c>
       <c r="E82" t="s">
-        <v>724</v>
+        <v>730</v>
       </c>
       <c r="F82" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G82" t="s">
-        <v>725</v>
+        <v>731</v>
       </c>
       <c r="H82" t="s">
-        <v>726</v>
+        <v>732</v>
       </c>
       <c r="I82" t="s">
         <v>238</v>
       </c>
       <c r="J82" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K82" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L82" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M82" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N82" t="s">
         <v>51</v>
@@ -7449,48 +7467,48 @@
       <c r="T82"/>
       <c r="U82"/>
       <c r="V82" t="s">
-        <v>727</v>
+        <v>733</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>728</v>
+        <v>734</v>
       </c>
       <c r="B83" t="s">
-        <v>729</v>
+        <v>735</v>
       </c>
       <c r="C83" t="s">
-        <v>730</v>
+        <v>736</v>
       </c>
       <c r="D83" t="s">
-        <v>731</v>
+        <v>737</v>
       </c>
       <c r="E83" t="s">
-        <v>731</v>
+        <v>737</v>
       </c>
       <c r="F83" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G83" t="s">
-        <v>732</v>
+        <v>738</v>
       </c>
       <c r="H83" t="s">
-        <v>733</v>
+        <v>739</v>
       </c>
       <c r="I83" t="s">
         <v>238</v>
       </c>
       <c r="J83" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K83" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L83" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M83" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N83" t="s">
         <v>51</v>
@@ -7505,48 +7523,48 @@
       <c r="T83"/>
       <c r="U83"/>
       <c r="V83" t="s">
-        <v>734</v>
+        <v>740</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>735</v>
+        <v>741</v>
       </c>
       <c r="B84" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c r="C84" t="s">
-        <v>737</v>
+        <v>743</v>
       </c>
       <c r="D84" t="s">
-        <v>738</v>
+        <v>744</v>
       </c>
       <c r="E84" t="s">
-        <v>738</v>
+        <v>744</v>
       </c>
       <c r="F84" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G84" t="s">
-        <v>739</v>
+        <v>745</v>
       </c>
       <c r="H84" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="I84" t="s">
         <v>238</v>
       </c>
       <c r="J84" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K84" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L84" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M84" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N84" t="s">
         <v>51</v>
@@ -7561,48 +7579,48 @@
       <c r="T84"/>
       <c r="U84"/>
       <c r="V84" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="B85" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="C85" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="D85" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="E85" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="F85" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G85" t="s">
-        <v>746</v>
+        <v>752</v>
       </c>
       <c r="H85" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="I85" t="s">
         <v>238</v>
       </c>
       <c r="J85" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K85" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L85" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M85" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N85" t="s">
         <v>51</v>
@@ -7617,48 +7635,48 @@
       <c r="T85"/>
       <c r="U85"/>
       <c r="V85" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="B86" t="s">
-        <v>750</v>
+        <v>756</v>
       </c>
       <c r="C86" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="D86" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="E86" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="F86" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G86" t="s">
-        <v>753</v>
+        <v>759</v>
       </c>
       <c r="H86" t="s">
-        <v>754</v>
+        <v>760</v>
       </c>
       <c r="I86" t="s">
         <v>238</v>
       </c>
       <c r="J86" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K86" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L86" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M86" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N86" t="s">
         <v>51</v>
@@ -7673,48 +7691,48 @@
       <c r="T86"/>
       <c r="U86"/>
       <c r="V86" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
       <c r="B87" t="s">
-        <v>757</v>
+        <v>763</v>
       </c>
       <c r="C87" t="s">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="D87" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="E87" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="F87" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G87" t="s">
-        <v>761</v>
+        <v>767</v>
       </c>
       <c r="H87" t="s">
-        <v>762</v>
+        <v>768</v>
       </c>
       <c r="I87" t="s">
         <v>238</v>
       </c>
       <c r="J87" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K87" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L87" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M87" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N87" t="s">
         <v>51</v>
@@ -7729,48 +7747,48 @@
       <c r="T87"/>
       <c r="U87"/>
       <c r="V87" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>764</v>
+        <v>770</v>
       </c>
       <c r="B88" t="s">
-        <v>765</v>
+        <v>771</v>
       </c>
       <c r="C88" t="s">
-        <v>766</v>
+        <v>772</v>
       </c>
       <c r="D88" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="E88" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="F88" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G88" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c r="H88" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="I88" t="s">
         <v>238</v>
       </c>
       <c r="J88" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K88" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L88" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M88" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N88" t="s">
         <v>51</v>
@@ -7785,48 +7803,48 @@
       <c r="T88"/>
       <c r="U88"/>
       <c r="V88" t="s">
-        <v>770</v>
+        <v>776</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
       <c r="B89" t="s">
-        <v>772</v>
+        <v>778</v>
       </c>
       <c r="C89" t="s">
-        <v>773</v>
+        <v>779</v>
       </c>
       <c r="D89" t="s">
-        <v>774</v>
+        <v>780</v>
       </c>
       <c r="E89" t="s">
-        <v>774</v>
+        <v>780</v>
       </c>
       <c r="F89" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G89" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="H89" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="I89" t="s">
         <v>238</v>
       </c>
       <c r="J89" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K89" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L89" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M89" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N89" t="s">
         <v>51</v>
@@ -7841,48 +7859,48 @@
       <c r="T89"/>
       <c r="U89"/>
       <c r="V89" t="s">
-        <v>777</v>
+        <v>783</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="B90" t="s">
-        <v>779</v>
+        <v>785</v>
       </c>
       <c r="C90" t="s">
-        <v>780</v>
+        <v>786</v>
       </c>
       <c r="D90" t="s">
-        <v>781</v>
+        <v>787</v>
       </c>
       <c r="E90" t="s">
-        <v>781</v>
+        <v>787</v>
       </c>
       <c r="F90" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G90" t="s">
-        <v>782</v>
+        <v>788</v>
       </c>
       <c r="H90" t="s">
-        <v>783</v>
+        <v>789</v>
       </c>
       <c r="I90" t="s">
         <v>238</v>
       </c>
       <c r="J90" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K90" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L90" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M90" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N90" t="s">
         <v>51</v>
@@ -7897,48 +7915,48 @@
       <c r="T90"/>
       <c r="U90"/>
       <c r="V90" t="s">
-        <v>784</v>
+        <v>790</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>785</v>
+        <v>791</v>
       </c>
       <c r="B91" t="s">
-        <v>786</v>
+        <v>792</v>
       </c>
       <c r="C91" t="s">
-        <v>787</v>
+        <v>793</v>
       </c>
       <c r="D91" t="s">
-        <v>788</v>
+        <v>794</v>
       </c>
       <c r="E91" t="s">
-        <v>788</v>
+        <v>794</v>
       </c>
       <c r="F91" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G91" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="H91" t="s">
-        <v>790</v>
+        <v>796</v>
       </c>
       <c r="I91" t="s">
         <v>238</v>
       </c>
       <c r="J91" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K91" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L91" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M91" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N91" t="s">
         <v>51</v>
@@ -7953,48 +7971,48 @@
       <c r="T91"/>
       <c r="U91"/>
       <c r="V91" t="s">
-        <v>791</v>
+        <v>797</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>792</v>
+        <v>798</v>
       </c>
       <c r="B92" t="s">
-        <v>793</v>
+        <v>799</v>
       </c>
       <c r="C92" t="s">
-        <v>794</v>
+        <v>800</v>
       </c>
       <c r="D92" t="s">
-        <v>795</v>
+        <v>801</v>
       </c>
       <c r="E92" t="s">
-        <v>795</v>
+        <v>801</v>
       </c>
       <c r="F92" t="s">
-        <v>706</v>
+        <v>712</v>
       </c>
       <c r="G92" t="s">
-        <v>796</v>
+        <v>802</v>
       </c>
       <c r="H92" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="I92" t="s">
         <v>238</v>
       </c>
       <c r="J92" t="s">
-        <v>709</v>
+        <v>715</v>
       </c>
       <c r="K92" t="s">
-        <v>710</v>
+        <v>716</v>
       </c>
       <c r="L92" t="s">
-        <v>711</v>
+        <v>717</v>
       </c>
       <c r="M92" t="s">
-        <v>712</v>
+        <v>718</v>
       </c>
       <c r="N92" t="s">
         <v>51</v>
@@ -8009,43 +8027,43 @@
       <c r="T92"/>
       <c r="U92"/>
       <c r="V92" t="s">
-        <v>797</v>
+        <v>803</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>798</v>
+        <v>804</v>
       </c>
       <c r="B93" t="s">
-        <v>799</v>
+        <v>805</v>
       </c>
       <c r="C93" t="s">
-        <v>800</v>
+        <v>806</v>
       </c>
       <c r="D93" t="s">
-        <v>801</v>
+        <v>807</v>
       </c>
       <c r="E93" t="s">
-        <v>802</v>
+        <v>808</v>
       </c>
       <c r="F93" t="s">
-        <v>803</v>
+        <v>809</v>
       </c>
       <c r="G93" t="s">
-        <v>803</v>
+        <v>809</v>
       </c>
       <c r="H93"/>
       <c r="I93" t="s">
         <v>28</v>
       </c>
       <c r="J93" t="s">
-        <v>804</v>
+        <v>810</v>
       </c>
       <c r="K93" t="s">
-        <v>805</v>
+        <v>811</v>
       </c>
       <c r="L93" t="s">
-        <v>806</v>
+        <v>812</v>
       </c>
       <c r="M93" t="s">
         <v>130</v>
@@ -8063,33 +8081,33 @@
       <c r="T93"/>
       <c r="U93"/>
       <c r="V93" t="s">
-        <v>807</v>
+        <v>813</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>808</v>
+        <v>814</v>
       </c>
       <c r="B94" t="s">
-        <v>809</v>
+        <v>815</v>
       </c>
       <c r="C94" t="s">
-        <v>810</v>
+        <v>816</v>
       </c>
       <c r="D94" t="s">
-        <v>811</v>
+        <v>817</v>
       </c>
       <c r="E94" t="s">
-        <v>811</v>
+        <v>817</v>
       </c>
       <c r="F94" t="s">
-        <v>812</v>
+        <v>818</v>
       </c>
       <c r="G94" t="s">
-        <v>813</v>
+        <v>819</v>
       </c>
       <c r="H94" t="s">
-        <v>814</v>
+        <v>820</v>
       </c>
       <c r="I94" t="s">
         <v>28</v>
@@ -8111,30 +8129,30 @@
       <c r="T94"/>
       <c r="U94"/>
       <c r="V94" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>816</v>
+        <v>822</v>
       </c>
       <c r="B95" t="s">
-        <v>817</v>
+        <v>823</v>
       </c>
       <c r="C95" t="s">
+        <v>824</v>
+      </c>
+      <c r="D95" t="s">
+        <v>825</v>
+      </c>
+      <c r="E95" t="s">
+        <v>825</v>
+      </c>
+      <c r="F95" t="s">
         <v>818</v>
       </c>
-      <c r="D95" t="s">
-        <v>819</v>
-      </c>
-      <c r="E95" t="s">
-        <v>819</v>
-      </c>
-      <c r="F95" t="s">
-        <v>812</v>
-      </c>
       <c r="G95" t="s">
-        <v>820</v>
+        <v>826</v>
       </c>
       <c r="H95"/>
       <c r="I95" t="s">
@@ -8157,30 +8175,30 @@
       <c r="T95"/>
       <c r="U95"/>
       <c r="V95" t="s">
-        <v>821</v>
+        <v>827</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>822</v>
+        <v>828</v>
       </c>
       <c r="B96" t="s">
-        <v>823</v>
+        <v>829</v>
       </c>
       <c r="C96" t="s">
-        <v>824</v>
+        <v>830</v>
       </c>
       <c r="D96" t="s">
-        <v>825</v>
+        <v>831</v>
       </c>
       <c r="E96" t="s">
-        <v>825</v>
+        <v>831</v>
       </c>
       <c r="F96" t="s">
         <v>25</v>
       </c>
       <c r="G96" t="s">
-        <v>826</v>
+        <v>832</v>
       </c>
       <c r="H96"/>
       <c r="I96" t="s">
@@ -8203,30 +8221,30 @@
       <c r="T96"/>
       <c r="U96"/>
       <c r="V96" t="s">
-        <v>827</v>
+        <v>833</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>828</v>
+        <v>834</v>
       </c>
       <c r="B97" t="s">
-        <v>829</v>
+        <v>835</v>
       </c>
       <c r="C97" t="s">
-        <v>830</v>
+        <v>836</v>
       </c>
       <c r="D97" t="s">
-        <v>831</v>
+        <v>837</v>
       </c>
       <c r="E97" t="s">
-        <v>831</v>
+        <v>837</v>
       </c>
       <c r="F97" t="s">
         <v>25</v>
       </c>
       <c r="G97" t="s">
-        <v>832</v>
+        <v>838</v>
       </c>
       <c r="H97"/>
       <c r="I97" t="s">
@@ -8249,30 +8267,30 @@
       <c r="T97"/>
       <c r="U97"/>
       <c r="V97" t="s">
-        <v>833</v>
+        <v>839</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>834</v>
+        <v>840</v>
       </c>
       <c r="B98" t="s">
-        <v>835</v>
+        <v>841</v>
       </c>
       <c r="C98" t="s">
-        <v>836</v>
+        <v>842</v>
       </c>
       <c r="D98" t="s">
-        <v>837</v>
+        <v>843</v>
       </c>
       <c r="E98" t="s">
-        <v>838</v>
+        <v>844</v>
       </c>
       <c r="F98" t="s">
         <v>25</v>
       </c>
       <c r="G98" t="s">
-        <v>839</v>
+        <v>845</v>
       </c>
       <c r="H98"/>
       <c r="I98" t="s">
@@ -8295,46 +8313,46 @@
       <c r="T98"/>
       <c r="U98"/>
       <c r="V98" t="s">
-        <v>840</v>
+        <v>846</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>841</v>
+        <v>847</v>
       </c>
       <c r="B99" t="s">
-        <v>842</v>
+        <v>848</v>
       </c>
       <c r="C99" t="s">
-        <v>843</v>
+        <v>849</v>
       </c>
       <c r="D99" t="s">
-        <v>844</v>
+        <v>850</v>
       </c>
       <c r="E99" t="s">
-        <v>845</v>
+        <v>851</v>
       </c>
       <c r="F99" t="s">
-        <v>846</v>
+        <v>852</v>
       </c>
       <c r="G99" t="s">
-        <v>847</v>
+        <v>853</v>
       </c>
       <c r="H99"/>
       <c r="I99" t="s">
         <v>28</v>
       </c>
       <c r="J99" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="K99" t="s">
-        <v>849</v>
+        <v>855</v>
       </c>
       <c r="L99" t="s">
-        <v>850</v>
+        <v>856</v>
       </c>
       <c r="M99" t="s">
-        <v>851</v>
+        <v>857</v>
       </c>
       <c r="N99" t="s">
         <v>51</v>
@@ -8349,46 +8367,46 @@
       <c r="T99"/>
       <c r="U99"/>
       <c r="V99" t="s">
-        <v>852</v>
+        <v>858</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>853</v>
+        <v>859</v>
       </c>
       <c r="B100" t="s">
-        <v>854</v>
+        <v>860</v>
       </c>
       <c r="C100" t="s">
-        <v>855</v>
+        <v>861</v>
       </c>
       <c r="D100" t="s">
-        <v>856</v>
+        <v>862</v>
       </c>
       <c r="E100" t="s">
-        <v>857</v>
+        <v>863</v>
       </c>
       <c r="F100" t="s">
-        <v>846</v>
+        <v>852</v>
       </c>
       <c r="G100" t="s">
-        <v>858</v>
+        <v>864</v>
       </c>
       <c r="H100"/>
       <c r="I100" t="s">
         <v>28</v>
       </c>
       <c r="J100" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="K100" t="s">
-        <v>849</v>
+        <v>855</v>
       </c>
       <c r="L100" t="s">
-        <v>850</v>
+        <v>856</v>
       </c>
       <c r="M100" t="s">
-        <v>851</v>
+        <v>857</v>
       </c>
       <c r="N100" t="s">
         <v>51</v>
@@ -8403,46 +8421,46 @@
       <c r="T100"/>
       <c r="U100"/>
       <c r="V100" t="s">
-        <v>859</v>
+        <v>865</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>860</v>
+        <v>866</v>
       </c>
       <c r="B101" t="s">
-        <v>861</v>
+        <v>867</v>
       </c>
       <c r="C101" t="s">
-        <v>862</v>
+        <v>868</v>
       </c>
       <c r="D101" t="s">
-        <v>863</v>
+        <v>869</v>
       </c>
       <c r="E101" t="s">
-        <v>864</v>
+        <v>870</v>
       </c>
       <c r="F101" t="s">
-        <v>846</v>
+        <v>852</v>
       </c>
       <c r="G101" t="s">
-        <v>865</v>
+        <v>871</v>
       </c>
       <c r="H101"/>
       <c r="I101" t="s">
         <v>28</v>
       </c>
       <c r="J101" t="s">
-        <v>848</v>
+        <v>854</v>
       </c>
       <c r="K101" t="s">
-        <v>849</v>
+        <v>855</v>
       </c>
       <c r="L101" t="s">
-        <v>850</v>
+        <v>856</v>
       </c>
       <c r="M101" t="s">
-        <v>851</v>
+        <v>857</v>
       </c>
       <c r="N101" t="s">
         <v>51</v>
@@ -8457,28 +8475,28 @@
       <c r="T101"/>
       <c r="U101"/>
       <c r="V101" t="s">
-        <v>866</v>
+        <v>872</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>867</v>
+        <v>873</v>
       </c>
       <c r="B102" t="s">
-        <v>868</v>
+        <v>874</v>
       </c>
       <c r="C102"/>
       <c r="D102" t="s">
-        <v>869</v>
+        <v>875</v>
       </c>
       <c r="E102" t="s">
-        <v>869</v>
+        <v>875</v>
       </c>
       <c r="F102" t="s">
-        <v>870</v>
+        <v>876</v>
       </c>
       <c r="G102" t="s">
-        <v>870</v>
+        <v>876</v>
       </c>
       <c r="H102"/>
       <c r="I102" t="s">
@@ -8501,26 +8519,26 @@
       <c r="T102"/>
       <c r="U102"/>
       <c r="V102" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>872</v>
+        <v>878</v>
       </c>
       <c r="B103" t="s">
-        <v>873</v>
+        <v>879</v>
       </c>
       <c r="C103" t="s">
         <v>76</v>
       </c>
       <c r="D103" t="s">
-        <v>874</v>
+        <v>880</v>
       </c>
       <c r="E103"/>
       <c r="F103"/>
       <c r="G103" t="s">
-        <v>873</v>
+        <v>879</v>
       </c>
       <c r="H103"/>
       <c r="I103"/>

</xml_diff>

<commit_message>
CIBER plots with short labels
</commit_message>
<xml_diff>
--- a/metadata/questionLabels.xlsx
+++ b/metadata/questionLabels.xlsx
@@ -878,10 +878,10 @@
     <t xml:space="preserve">7 Täysin automaattista</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Not at all automatic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 Fully automatic</t>
+    <t xml:space="preserve">Not at all automatic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fully automatic</t>
   </si>
   <si>
     <t xml:space="preserve">automaticity_carry_mask = Q13_1,</t>

</xml_diff>